<commit_message>
Classes interagem umas com as outras Falta a implementação da classe
</commit_message>
<xml_diff>
--- a/ES-2Sem-2021-Grupo6/temp.xlsx
+++ b/ES-2Sem-2021-Grupo6/temp.xlsx
@@ -6,21 +6,45 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Persons" r:id="rId3" sheetId="1"/>
+    <sheet name="Results" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Name</t>
+    <t>MethodID</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>Package</t>
   </si>
   <si>
-    <t>John Smith</t>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>NOM_Class</t>
+  </si>
+  <si>
+    <t>LOC_Class</t>
+  </si>
+  <si>
+    <t>WMC_Class</t>
+  </si>
+  <si>
+    <t>is_God_Class</t>
+  </si>
+  <si>
+    <t>LOC_Method</t>
+  </si>
+  <si>
+    <t>CYCLO_Method</t>
+  </si>
+  <si>
+    <t>is_Long_Method</t>
   </si>
 </sst>
 </file>
@@ -42,22 +66,12 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="48"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="48"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,7 +88,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -90,8 +104,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="23.4375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
+    <col min="1" max="1" width="11.71875" customWidth="true"/>
+    <col min="2" max="2" width="11.71875" customWidth="true"/>
+    <col min="3" max="3" width="23.4375" customWidth="true"/>
+    <col min="4" max="4" width="31.25" customWidth="true"/>
+    <col min="5" max="5" width="11.71875" customWidth="true"/>
+    <col min="6" max="6" width="11.71875" customWidth="true"/>
+    <col min="7" max="7" width="11.71875" customWidth="true"/>
+    <col min="8" max="8" width="11.71875" customWidth="true"/>
+    <col min="9" max="9" width="11.71875" customWidth="true"/>
+    <col min="10" max="10" width="11.71875" customWidth="true"/>
+    <col min="11" max="11" width="11.71875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -101,13 +124,32 @@
       <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="n" s="2">
-        <v>20.0</v>
+      <c r="D1" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>